<commit_message>
muda de pygame para flask
</commit_message>
<xml_diff>
--- a/Dados_Iluminator.xlsx
+++ b/Dados_Iluminator.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA30"/>
+  <dimension ref="A1:BA35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,257 +422,257 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>pessoa</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>mulher</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>professor</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>filhos</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>c_materia</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>c_vida</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>c_humanas</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>c_dados</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>mais_24_anos</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>russo</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>gatos</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>barba</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>oculos</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>bordao</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>maquina</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>ilum</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>laboratorio</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>pelucia</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>3d</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>aluno</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>estagiario</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>funcionario</t>
         </is>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" t="n">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" t="n">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" t="n">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" t="n">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" t="n">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>experimental</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>adotado</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>luggo</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>v2</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>v3</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>v4</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>volei</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>futebol</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>tecnico</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>alto</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>baixo</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>cabelo_longo</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>cabelo_curto</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>cabelo_cacheado</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>cabelo_liso</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>branco</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>preto</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>camisa</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>moto</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>bone</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>tarot</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>teorico</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>colorido</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>atletica</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>ca</t>
         </is>
@@ -1192,22 +1180,22 @@
         <v>-10</v>
       </c>
       <c r="D5" t="n">
-        <v>11.9</v>
+        <v>14.75</v>
       </c>
       <c r="E5" t="n">
         <v>-10</v>
       </c>
       <c r="F5" t="n">
-        <v>11.9</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>-10</v>
+        <v>-12.85</v>
       </c>
       <c r="H5" t="n">
         <v>-10</v>
       </c>
       <c r="I5" t="n">
-        <v>10</v>
+        <v>12.85</v>
       </c>
       <c r="J5" t="n">
         <v>10</v>
@@ -1219,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>10</v>
+        <v>12.85</v>
       </c>
       <c r="N5" t="n">
-        <v>11.9</v>
+        <v>14.75</v>
       </c>
       <c r="O5" t="n">
         <v>11.9</v>
@@ -4935,13 +4923,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.95</v>
+        <v>1.9</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>-0.95</v>
       </c>
       <c r="D28" t="n">
-        <v>-1.9</v>
+        <v>-2.85</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -4950,7 +4938,7 @@
         <v>-1.9</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>-0.95</v>
       </c>
       <c r="H28" t="n">
         <v>-0.95</v>
@@ -4959,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>-1.9</v>
+        <v>-2.85</v>
       </c>
       <c r="K28" t="n">
         <v>0</v>
@@ -4971,7 +4959,7 @@
         <v>-0.95</v>
       </c>
       <c r="N28" t="n">
-        <v>1.9</v>
+        <v>2.85</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
@@ -4983,58 +4971,58 @@
         <v>0</v>
       </c>
       <c r="R28" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>-0.95</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI28" t="n">
         <v>0.75</v>
-      </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" t="n">
-        <v>0</v>
-      </c>
-      <c r="U28" t="n">
-        <v>0</v>
-      </c>
-      <c r="V28" t="n">
-        <v>0</v>
-      </c>
-      <c r="W28" t="n">
-        <v>0</v>
-      </c>
-      <c r="X28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI28" t="n">
-        <v>0</v>
       </c>
       <c r="AJ28" t="n">
         <v>0</v>
@@ -5415,6 +5403,821 @@
       </c>
       <c r="BA30" t="n">
         <v>-0.95</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Bruna (T26)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-4.75</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>-4.75</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="L31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="M31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="N31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="O31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="P31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="R31" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="S31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="T31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="U31" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="V31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="W31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="X31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>-4.75</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="AV31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ31" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="BA31" t="n">
+        <v>-3.8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ricardo (T26)</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-2.85</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="L32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="M32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="N32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="O32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="P32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="R32" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="S32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="T32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="U32" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="V32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="W32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="X32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>-2.85</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>-0.95</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>-1.15</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="AV32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ32" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="BA32" t="n">
+        <v>-1.9</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA35" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
muda o tipo de sessão para REDIS
</commit_message>
<xml_diff>
--- a/Dados_Iluminator.xlsx
+++ b/Dados_Iluminator.xlsx
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>-10</v>
+        <v>-10.95</v>
       </c>
       <c r="D5" t="n">
         <v>14.75</v>
@@ -1186,19 +1186,19 @@
         <v>-10</v>
       </c>
       <c r="F5" t="n">
-        <v>9.050000000000001</v>
+        <v>8.100000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>-12.85</v>
+        <v>-13.8</v>
       </c>
       <c r="H5" t="n">
         <v>-10</v>
       </c>
       <c r="I5" t="n">
-        <v>12.85</v>
+        <v>13.8</v>
       </c>
       <c r="J5" t="n">
-        <v>10</v>
+        <v>10.95</v>
       </c>
       <c r="K5" t="n">
         <v>-10</v>
@@ -1210,7 +1210,7 @@
         <v>12.85</v>
       </c>
       <c r="N5" t="n">
-        <v>14.75</v>
+        <v>15.7</v>
       </c>
       <c r="O5" t="n">
         <v>11.9</v>

</xml_diff>